<commit_message>
Deployed a111169 with MkDocs version: 1.4.3
</commit_message>
<xml_diff>
--- a/moody-s_datahub/moodys_datahub/data/data_products.xlsx
+++ b/moody-s_datahub/moodys_datahub/data/data_products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/kgp_lib_cbs_dk/Documents/Desktop/moody-s_datahub/moodys_datahub/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="11_4B0D37945B70D6289F9A3B11595ED87656CCA927" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5434116-813D-4DE2-8AB8-C734A0F3D298}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="11_4B0D37945B70D6289F9A3B11595ED87656CCA927" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A369D3B-379B-4624-9B9F-A13AC10ED3C9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="183">
   <si>
     <t>Data Product</t>
   </si>
@@ -560,6 +560,18 @@
   </si>
   <si>
     <t>mqO4CUwDQYW8IVCJRaJJ7Q</t>
+  </si>
+  <si>
+    <t>BvD ID Changes</t>
+  </si>
+  <si>
+    <t>AchNv9QQS0qFrThlyqXhDw</t>
+  </si>
+  <si>
+    <t>d1uBZqfHSLOhAmhZWTDySw</t>
+  </si>
+  <si>
+    <t>bvd_id_changes_full</t>
   </si>
 </sst>
 </file>
@@ -940,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E299"/>
+  <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3505,16 +3517,16 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="C151" t="s">
-        <v>60</v>
+        <v>182</v>
       </c>
       <c r="D151" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="E151" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3525,7 +3537,7 @@
         <v>145</v>
       </c>
       <c r="C152" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D152" t="s">
         <v>159</v>
@@ -3539,13 +3551,13 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="C153" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D153" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E153" t="s">
         <v>176</v>
@@ -3559,7 +3571,7 @@
         <v>111</v>
       </c>
       <c r="C154" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D154" t="s">
         <v>160</v>
@@ -3576,7 +3588,7 @@
         <v>111</v>
       </c>
       <c r="C155" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D155" t="s">
         <v>160</v>
@@ -3590,13 +3602,13 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C156" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="D156" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E156" t="s">
         <v>176</v>
@@ -3610,7 +3622,7 @@
         <v>113</v>
       </c>
       <c r="C157" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D157" t="s">
         <v>161</v>
@@ -3627,7 +3639,7 @@
         <v>113</v>
       </c>
       <c r="C158" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D158" t="s">
         <v>161</v>
@@ -3644,7 +3656,7 @@
         <v>113</v>
       </c>
       <c r="C159" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D159" t="s">
         <v>161</v>
@@ -3661,7 +3673,7 @@
         <v>113</v>
       </c>
       <c r="C160" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D160" t="s">
         <v>161</v>
@@ -3678,7 +3690,7 @@
         <v>113</v>
       </c>
       <c r="C161" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D161" t="s">
         <v>161</v>
@@ -3692,13 +3704,13 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="C162" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="D162" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E162" t="s">
         <v>176</v>
@@ -3712,7 +3724,7 @@
         <v>68</v>
       </c>
       <c r="C163" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D163" t="s">
         <v>162</v>
@@ -3729,7 +3741,7 @@
         <v>68</v>
       </c>
       <c r="C164" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D164" t="s">
         <v>162</v>
@@ -3746,7 +3758,7 @@
         <v>68</v>
       </c>
       <c r="C165" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D165" t="s">
         <v>162</v>
@@ -3763,7 +3775,7 @@
         <v>68</v>
       </c>
       <c r="C166" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D166" t="s">
         <v>162</v>
@@ -3780,7 +3792,7 @@
         <v>68</v>
       </c>
       <c r="C167" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D167" t="s">
         <v>162</v>
@@ -3797,7 +3809,7 @@
         <v>68</v>
       </c>
       <c r="C168" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D168" t="s">
         <v>162</v>
@@ -3814,7 +3826,7 @@
         <v>68</v>
       </c>
       <c r="C169" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D169" t="s">
         <v>162</v>
@@ -3831,7 +3843,7 @@
         <v>68</v>
       </c>
       <c r="C170" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D170" t="s">
         <v>162</v>
@@ -3848,7 +3860,7 @@
         <v>68</v>
       </c>
       <c r="C171" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D171" t="s">
         <v>162</v>
@@ -3865,7 +3877,7 @@
         <v>68</v>
       </c>
       <c r="C172" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D172" t="s">
         <v>162</v>
@@ -3882,7 +3894,7 @@
         <v>68</v>
       </c>
       <c r="C173" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D173" t="s">
         <v>162</v>
@@ -3899,7 +3911,7 @@
         <v>68</v>
       </c>
       <c r="C174" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D174" t="s">
         <v>162</v>
@@ -3916,7 +3928,7 @@
         <v>68</v>
       </c>
       <c r="C175" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D175" t="s">
         <v>162</v>
@@ -3933,7 +3945,7 @@
         <v>68</v>
       </c>
       <c r="C176" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D176" t="s">
         <v>162</v>
@@ -3950,7 +3962,7 @@
         <v>68</v>
       </c>
       <c r="C177" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D177" t="s">
         <v>162</v>
@@ -3967,7 +3979,7 @@
         <v>68</v>
       </c>
       <c r="C178" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D178" t="s">
         <v>162</v>
@@ -3984,7 +3996,7 @@
         <v>68</v>
       </c>
       <c r="C179" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D179" t="s">
         <v>162</v>
@@ -3998,13 +4010,13 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="C180" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="D180" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E180" t="s">
         <v>176</v>
@@ -4015,13 +4027,13 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="C181" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="D181" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E181" t="s">
         <v>176</v>
@@ -4035,7 +4047,7 @@
         <v>99</v>
       </c>
       <c r="C182" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D182" t="s">
         <v>164</v>
@@ -4052,7 +4064,7 @@
         <v>99</v>
       </c>
       <c r="C183" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D183" t="s">
         <v>164</v>
@@ -4069,7 +4081,7 @@
         <v>99</v>
       </c>
       <c r="C184" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D184" t="s">
         <v>164</v>
@@ -4083,13 +4095,13 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="C185" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="D185" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E185" t="s">
         <v>176</v>
@@ -4103,7 +4115,7 @@
         <v>3</v>
       </c>
       <c r="C186" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D186" t="s">
         <v>165</v>
@@ -4120,7 +4132,7 @@
         <v>3</v>
       </c>
       <c r="C187" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D187" t="s">
         <v>165</v>
@@ -4137,7 +4149,7 @@
         <v>3</v>
       </c>
       <c r="C188" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D188" t="s">
         <v>165</v>
@@ -4154,7 +4166,7 @@
         <v>3</v>
       </c>
       <c r="C189" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D189" t="s">
         <v>165</v>
@@ -4171,7 +4183,7 @@
         <v>3</v>
       </c>
       <c r="C190" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D190" t="s">
         <v>165</v>
@@ -4188,7 +4200,7 @@
         <v>3</v>
       </c>
       <c r="C191" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D191" t="s">
         <v>165</v>
@@ -4205,7 +4217,7 @@
         <v>3</v>
       </c>
       <c r="C192" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D192" t="s">
         <v>165</v>
@@ -4222,7 +4234,7 @@
         <v>3</v>
       </c>
       <c r="C193" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D193" t="s">
         <v>165</v>
@@ -4239,7 +4251,7 @@
         <v>3</v>
       </c>
       <c r="C194" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D194" t="s">
         <v>165</v>
@@ -4253,13 +4265,13 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="C195" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="D195" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E195" t="s">
         <v>176</v>
@@ -4273,7 +4285,7 @@
         <v>91</v>
       </c>
       <c r="C196" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D196" t="s">
         <v>166</v>
@@ -4290,7 +4302,7 @@
         <v>91</v>
       </c>
       <c r="C197" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D197" t="s">
         <v>166</v>
@@ -4307,7 +4319,7 @@
         <v>91</v>
       </c>
       <c r="C198" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D198" t="s">
         <v>166</v>
@@ -4324,7 +4336,7 @@
         <v>91</v>
       </c>
       <c r="C199" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D199" t="s">
         <v>166</v>
@@ -4341,7 +4353,7 @@
         <v>91</v>
       </c>
       <c r="C200" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D200" t="s">
         <v>166</v>
@@ -4355,13 +4367,13 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="C201" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="D201" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E201" t="s">
         <v>176</v>
@@ -4375,7 +4387,7 @@
         <v>49</v>
       </c>
       <c r="C202" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D202" t="s">
         <v>167</v>
@@ -4392,7 +4404,7 @@
         <v>49</v>
       </c>
       <c r="C203" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D203" t="s">
         <v>167</v>
@@ -4409,7 +4421,7 @@
         <v>49</v>
       </c>
       <c r="C204" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D204" t="s">
         <v>167</v>
@@ -4426,7 +4438,7 @@
         <v>49</v>
       </c>
       <c r="C205" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D205" t="s">
         <v>167</v>
@@ -4443,7 +4455,7 @@
         <v>49</v>
       </c>
       <c r="C206" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D206" t="s">
         <v>167</v>
@@ -4460,7 +4472,7 @@
         <v>49</v>
       </c>
       <c r="C207" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D207" t="s">
         <v>167</v>
@@ -4477,7 +4489,7 @@
         <v>49</v>
       </c>
       <c r="C208" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D208" t="s">
         <v>167</v>
@@ -4494,7 +4506,7 @@
         <v>49</v>
       </c>
       <c r="C209" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D209" t="s">
         <v>167</v>
@@ -4508,13 +4520,13 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>140</v>
+        <v>49</v>
       </c>
       <c r="C210" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="D210" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E210" t="s">
         <v>176</v>
@@ -4528,7 +4540,7 @@
         <v>140</v>
       </c>
       <c r="C211" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D211" t="s">
         <v>168</v>
@@ -4545,7 +4557,7 @@
         <v>140</v>
       </c>
       <c r="C212" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D212" t="s">
         <v>168</v>
@@ -4562,7 +4574,7 @@
         <v>140</v>
       </c>
       <c r="C213" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D213" t="s">
         <v>168</v>
@@ -4579,7 +4591,7 @@
         <v>140</v>
       </c>
       <c r="C214" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D214" t="s">
         <v>168</v>
@@ -4593,13 +4605,13 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="C215" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="D215" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E215" t="s">
         <v>176</v>
@@ -4610,13 +4622,13 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>144</v>
+        <v>88</v>
       </c>
       <c r="C216" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="D216" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E216" t="s">
         <v>176</v>
@@ -4630,7 +4642,7 @@
         <v>144</v>
       </c>
       <c r="C217" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D217" t="s">
         <v>170</v>
@@ -4647,7 +4659,7 @@
         <v>144</v>
       </c>
       <c r="C218" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D218" t="s">
         <v>170</v>
@@ -4664,7 +4676,7 @@
         <v>144</v>
       </c>
       <c r="C219" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D219" t="s">
         <v>170</v>
@@ -4681,7 +4693,7 @@
         <v>144</v>
       </c>
       <c r="C220" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D220" t="s">
         <v>170</v>
@@ -4698,7 +4710,7 @@
         <v>144</v>
       </c>
       <c r="C221" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D221" t="s">
         <v>170</v>
@@ -4715,7 +4727,7 @@
         <v>144</v>
       </c>
       <c r="C222" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D222" t="s">
         <v>170</v>
@@ -4732,7 +4744,7 @@
         <v>144</v>
       </c>
       <c r="C223" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D223" t="s">
         <v>170</v>
@@ -4749,7 +4761,7 @@
         <v>144</v>
       </c>
       <c r="C224" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D224" t="s">
         <v>170</v>
@@ -4766,7 +4778,7 @@
         <v>144</v>
       </c>
       <c r="C225" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D225" t="s">
         <v>170</v>
@@ -4780,13 +4792,13 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C226" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="D226" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E226" t="s">
         <v>176</v>
@@ -4800,7 +4812,7 @@
         <v>64</v>
       </c>
       <c r="C227" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D227" t="s">
         <v>171</v>
@@ -4814,13 +4826,13 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>139</v>
+        <v>64</v>
       </c>
       <c r="C228" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="D228" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E228" t="s">
         <v>176</v>
@@ -4834,7 +4846,7 @@
         <v>139</v>
       </c>
       <c r="C229" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D229" t="s">
         <v>172</v>
@@ -4851,7 +4863,7 @@
         <v>139</v>
       </c>
       <c r="C230" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D230" t="s">
         <v>172</v>
@@ -4868,7 +4880,7 @@
         <v>139</v>
       </c>
       <c r="C231" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D231" t="s">
         <v>172</v>
@@ -4885,7 +4897,7 @@
         <v>139</v>
       </c>
       <c r="C232" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D232" t="s">
         <v>172</v>
@@ -4902,7 +4914,7 @@
         <v>139</v>
       </c>
       <c r="C233" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D233" t="s">
         <v>172</v>
@@ -4919,7 +4931,7 @@
         <v>139</v>
       </c>
       <c r="C234" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D234" t="s">
         <v>172</v>
@@ -4936,7 +4948,7 @@
         <v>139</v>
       </c>
       <c r="C235" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D235" t="s">
         <v>172</v>
@@ -4953,7 +4965,7 @@
         <v>139</v>
       </c>
       <c r="C236" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D236" t="s">
         <v>172</v>
@@ -4970,7 +4982,7 @@
         <v>139</v>
       </c>
       <c r="C237" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D237" t="s">
         <v>172</v>
@@ -4987,7 +4999,7 @@
         <v>139</v>
       </c>
       <c r="C238" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D238" t="s">
         <v>172</v>
@@ -5004,7 +5016,7 @@
         <v>139</v>
       </c>
       <c r="C239" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D239" t="s">
         <v>172</v>
@@ -5021,7 +5033,7 @@
         <v>139</v>
       </c>
       <c r="C240" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D240" t="s">
         <v>172</v>
@@ -5038,7 +5050,7 @@
         <v>139</v>
       </c>
       <c r="C241" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D241" t="s">
         <v>172</v>
@@ -5055,7 +5067,7 @@
         <v>139</v>
       </c>
       <c r="C242" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D242" t="s">
         <v>172</v>
@@ -5069,13 +5081,13 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C243" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D243" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E243" t="s">
         <v>176</v>
@@ -5089,7 +5101,7 @@
         <v>142</v>
       </c>
       <c r="C244" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D244" t="s">
         <v>173</v>
@@ -5106,7 +5118,7 @@
         <v>142</v>
       </c>
       <c r="C245" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D245" t="s">
         <v>173</v>
@@ -5123,7 +5135,7 @@
         <v>142</v>
       </c>
       <c r="C246" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D246" t="s">
         <v>173</v>
@@ -5140,7 +5152,7 @@
         <v>142</v>
       </c>
       <c r="C247" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D247" t="s">
         <v>173</v>
@@ -5157,7 +5169,7 @@
         <v>142</v>
       </c>
       <c r="C248" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D248" t="s">
         <v>173</v>
@@ -5174,7 +5186,7 @@
         <v>142</v>
       </c>
       <c r="C249" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D249" t="s">
         <v>173</v>
@@ -5191,7 +5203,7 @@
         <v>142</v>
       </c>
       <c r="C250" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D250" t="s">
         <v>173</v>
@@ -5208,7 +5220,7 @@
         <v>142</v>
       </c>
       <c r="C251" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D251" t="s">
         <v>173</v>
@@ -5225,7 +5237,7 @@
         <v>142</v>
       </c>
       <c r="C252" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D252" t="s">
         <v>173</v>
@@ -5242,7 +5254,7 @@
         <v>142</v>
       </c>
       <c r="C253" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D253" t="s">
         <v>173</v>
@@ -5259,7 +5271,7 @@
         <v>142</v>
       </c>
       <c r="C254" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D254" t="s">
         <v>173</v>
@@ -5273,13 +5285,13 @@
         <v>254</v>
       </c>
       <c r="B255" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C255" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D255" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E255" t="s">
         <v>176</v>
@@ -5293,7 +5305,7 @@
         <v>143</v>
       </c>
       <c r="C256" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D256" t="s">
         <v>174</v>
@@ -5310,7 +5322,7 @@
         <v>143</v>
       </c>
       <c r="C257" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D257" t="s">
         <v>174</v>
@@ -5327,7 +5339,7 @@
         <v>143</v>
       </c>
       <c r="C258" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D258" t="s">
         <v>174</v>
@@ -5344,7 +5356,7 @@
         <v>143</v>
       </c>
       <c r="C259" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D259" t="s">
         <v>174</v>
@@ -5361,7 +5373,7 @@
         <v>143</v>
       </c>
       <c r="C260" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D260" t="s">
         <v>174</v>
@@ -5378,7 +5390,7 @@
         <v>143</v>
       </c>
       <c r="C261" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D261" t="s">
         <v>174</v>
@@ -5395,7 +5407,7 @@
         <v>143</v>
       </c>
       <c r="C262" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D262" t="s">
         <v>174</v>
@@ -5412,7 +5424,7 @@
         <v>143</v>
       </c>
       <c r="C263" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D263" t="s">
         <v>174</v>
@@ -5426,13 +5438,13 @@
         <v>263</v>
       </c>
       <c r="B264" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C264" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D264" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E264" t="s">
         <v>176</v>
@@ -5446,7 +5458,7 @@
         <v>141</v>
       </c>
       <c r="C265" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="D265" t="s">
         <v>175</v>
@@ -5463,7 +5475,7 @@
         <v>141</v>
       </c>
       <c r="C266" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D266" t="s">
         <v>175</v>
@@ -5480,7 +5492,7 @@
         <v>141</v>
       </c>
       <c r="C267" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D267" t="s">
         <v>175</v>
@@ -5497,7 +5509,7 @@
         <v>141</v>
       </c>
       <c r="C268" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D268" t="s">
         <v>175</v>
@@ -5514,7 +5526,7 @@
         <v>141</v>
       </c>
       <c r="C269" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D269" t="s">
         <v>175</v>
@@ -5531,7 +5543,7 @@
         <v>141</v>
       </c>
       <c r="C270" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D270" t="s">
         <v>175</v>
@@ -5548,7 +5560,7 @@
         <v>141</v>
       </c>
       <c r="C271" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D271" t="s">
         <v>175</v>
@@ -5565,7 +5577,7 @@
         <v>141</v>
       </c>
       <c r="C272" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D272" t="s">
         <v>175</v>
@@ -5582,7 +5594,7 @@
         <v>141</v>
       </c>
       <c r="C273" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D273" t="s">
         <v>175</v>
@@ -5599,7 +5611,7 @@
         <v>141</v>
       </c>
       <c r="C274" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D274" t="s">
         <v>175</v>
@@ -5616,7 +5628,7 @@
         <v>141</v>
       </c>
       <c r="C275" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D275" t="s">
         <v>175</v>
@@ -5633,7 +5645,7 @@
         <v>141</v>
       </c>
       <c r="C276" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D276" t="s">
         <v>175</v>
@@ -5650,7 +5662,7 @@
         <v>141</v>
       </c>
       <c r="C277" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D277" t="s">
         <v>175</v>
@@ -5667,7 +5679,7 @@
         <v>141</v>
       </c>
       <c r="C278" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D278" t="s">
         <v>175</v>
@@ -5684,7 +5696,7 @@
         <v>141</v>
       </c>
       <c r="C279" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D279" t="s">
         <v>175</v>
@@ -5701,7 +5713,7 @@
         <v>141</v>
       </c>
       <c r="C280" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D280" t="s">
         <v>175</v>
@@ -5718,7 +5730,7 @@
         <v>141</v>
       </c>
       <c r="C281" t="s">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="D281" t="s">
         <v>175</v>
@@ -5732,13 +5744,13 @@
         <v>281</v>
       </c>
       <c r="B282" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C282" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="D282" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E282" t="s">
         <v>176</v>
@@ -5752,7 +5764,7 @@
         <v>146</v>
       </c>
       <c r="C283" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D283" t="s">
         <v>177</v>
@@ -5769,7 +5781,7 @@
         <v>146</v>
       </c>
       <c r="C284" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D284" t="s">
         <v>177</v>
@@ -5786,7 +5798,7 @@
         <v>146</v>
       </c>
       <c r="C285" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D285" t="s">
         <v>177</v>
@@ -5803,7 +5815,7 @@
         <v>146</v>
       </c>
       <c r="C286" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D286" t="s">
         <v>177</v>
@@ -5820,7 +5832,7 @@
         <v>146</v>
       </c>
       <c r="C287" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D287" t="s">
         <v>177</v>
@@ -5837,7 +5849,7 @@
         <v>146</v>
       </c>
       <c r="C288" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D288" t="s">
         <v>177</v>
@@ -5854,7 +5866,7 @@
         <v>146</v>
       </c>
       <c r="C289" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D289" t="s">
         <v>177</v>
@@ -5871,7 +5883,7 @@
         <v>146</v>
       </c>
       <c r="C290" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D290" t="s">
         <v>177</v>
@@ -5885,13 +5897,13 @@
         <v>290</v>
       </c>
       <c r="B291" t="s">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="C291" t="s">
-        <v>148</v>
+        <v>44</v>
       </c>
       <c r="D291" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E291" t="s">
         <v>176</v>
@@ -5905,7 +5917,7 @@
         <v>34</v>
       </c>
       <c r="C292" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D292" t="s">
         <v>178</v>
@@ -5922,7 +5934,7 @@
         <v>34</v>
       </c>
       <c r="C293" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D293" t="s">
         <v>178</v>
@@ -5939,7 +5951,7 @@
         <v>34</v>
       </c>
       <c r="C294" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D294" t="s">
         <v>178</v>
@@ -5956,7 +5968,7 @@
         <v>34</v>
       </c>
       <c r="C295" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D295" t="s">
         <v>178</v>
@@ -5973,7 +5985,7 @@
         <v>34</v>
       </c>
       <c r="C296" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D296" t="s">
         <v>178</v>
@@ -5990,7 +6002,7 @@
         <v>34</v>
       </c>
       <c r="C297" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D297" t="s">
         <v>178</v>
@@ -6007,7 +6019,7 @@
         <v>34</v>
       </c>
       <c r="C298" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D298" t="s">
         <v>178</v>
@@ -6024,7 +6036,7 @@
         <v>34</v>
       </c>
       <c r="C299" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D299" t="s">
         <v>178</v>
@@ -6033,8 +6045,46 @@
         <v>176</v>
       </c>
     </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>299</v>
+      </c>
+      <c r="B300" t="s">
+        <v>34</v>
+      </c>
+      <c r="C300" t="s">
+        <v>156</v>
+      </c>
+      <c r="D300" t="s">
+        <v>178</v>
+      </c>
+      <c r="E300" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>300</v>
+      </c>
+      <c r="B301" t="s">
+        <v>179</v>
+      </c>
+      <c r="C301" t="s">
+        <v>182</v>
+      </c>
+      <c r="D301" t="s">
+        <v>180</v>
+      </c>
+      <c r="E301" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E301">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>